<commit_message>
Added demo flights / bookings
</commit_message>
<xml_diff>
--- a/csv_data/bookings.xlsx
+++ b/csv_data/bookings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/nicolas_caviezel_accenture_com/Documents/sujets/chat_w_doc_demo/csv_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{17760D0C-29D4-884C-B34E-D6C10AC65340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1DF3FBA-9A67-9245-926F-CC0AC3FEC84F}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{17760D0C-29D4-884C-B34E-D6C10AC65340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B1BA73-E656-D74D-B47B-EA30ADAD030C}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="960" windowWidth="16980" windowHeight="9780" xr2:uid="{9809AAE1-C816-454E-9672-02BB1AE4699A}"/>
+    <workbookView xWindow="17380" yWindow="960" windowWidth="16980" windowHeight="9780" xr2:uid="{9809AAE1-C816-454E-9672-02BB1AE4699A}"/>
   </bookViews>
   <sheets>
     <sheet name="bookings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>booking_id</t>
   </si>
@@ -65,61 +65,31 @@
     <t>AMS</t>
   </si>
   <si>
-    <t>JFK</t>
-  </si>
-  <si>
-    <t>ON TIME</t>
-  </si>
-  <si>
-    <t>Caviezel</t>
-  </si>
-  <si>
-    <t>Nicolas</t>
-  </si>
-  <si>
     <t>CDG</t>
   </si>
   <si>
-    <t>VCE</t>
-  </si>
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>Slama</t>
-  </si>
-  <si>
-    <t>TLV</t>
-  </si>
-  <si>
     <t>DELAYED</t>
   </si>
   <si>
-    <t>Julie</t>
-  </si>
-  <si>
-    <t>Lestienne</t>
-  </si>
-  <si>
-    <t>Nce</t>
-  </si>
-  <si>
     <t>passport_id</t>
   </si>
   <si>
-    <t>123AZD1</t>
-  </si>
-  <si>
-    <t>189ADZ</t>
-  </si>
-  <si>
-    <t>AZD123</t>
-  </si>
-  <si>
-    <t>INO23R</t>
-  </si>
-  <si>
     <t>Koenigs</t>
+  </si>
+  <si>
+    <t>Myrthe</t>
+  </si>
+  <si>
+    <t>Polfliet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON TIME </t>
+  </si>
+  <si>
+    <t>FCO</t>
+  </si>
+  <si>
+    <t>BCN</t>
   </si>
 </sst>
 </file>
@@ -479,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7318EE9B-78FC-7C4A-A890-72271BC4F6E2}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,18 +485,18 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -540,112 +510,138 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>23</v>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1">
-        <v>45272</v>
+        <v>45275</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="1">
-        <v>45275</v>
+        <v>45277</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
-        <v>45285</v>
+        <v>45283</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45301</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45277</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45320</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>